<commit_message>
PDS V1.3 DMA BIEN6
</commit_message>
<xml_diff>
--- a/STM32F051C8T6/MIS PROYECTOS/PORTABLE DIGITAL SOURCE V1.3 DMA/DESIGN POWER3.xlsx
+++ b/STM32F051C8T6/MIS PROYECTOS/PORTABLE DIGITAL SOURCE V1.3 DMA/DESIGN POWER3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIOVANNY_TODO\SKETCHS\STM32\STM32F051C8T6\MIS PROYECTOS\PORTABLE DIGITAL SOURCE V1.3 DMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBA9BDE-77E6-4945-8815-E881ED21EC1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F6C0EF-F02B-450C-92A5-74E6992C75EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97884494-F9FC-454E-B7F0-C1DF6E6FC067}"/>
   </bookViews>
@@ -1453,6 +1453,386 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-PE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$F$252:$F$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$G$252:$G$259</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3392-49F9-BE21-23F3B66D58C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="166230016"/>
+        <c:axId val="165899840"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="166230016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="165899840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="165899840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166230016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1533,6 +1913,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2050,6 +2470,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3031,6 +3967,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>236</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87212DC3-2CF3-4614-9FC4-4A271647C1FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3331,10 +4303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D153B7-22F3-48BB-9E72-85FF6508B366}">
-  <dimension ref="B6:Y238"/>
+  <dimension ref="B6:Y259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N211" sqref="N211"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G241" sqref="G241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6315,6 +7287,146 @@
         <v>43</v>
       </c>
     </row>
+    <row r="241" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F242">
+        <v>1.8</v>
+      </c>
+      <c r="G242">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="243" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F243">
+        <v>3.3</v>
+      </c>
+      <c r="G243">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="244" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F244">
+        <v>5</v>
+      </c>
+      <c r="G244">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="245" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F245">
+        <v>9</v>
+      </c>
+      <c r="G245">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="246" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F246">
+        <v>12</v>
+      </c>
+      <c r="G246">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="247" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F247">
+        <v>15</v>
+      </c>
+      <c r="G247">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="248" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F248">
+        <v>24</v>
+      </c>
+      <c r="G248">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="249" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F249">
+        <v>30</v>
+      </c>
+      <c r="G249">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F252">
+        <v>2.5</v>
+      </c>
+      <c r="G252">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="253" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F253">
+        <v>3.8</v>
+      </c>
+      <c r="G253">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="254" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F254">
+        <v>7</v>
+      </c>
+      <c r="G254">
+        <v>2000</v>
+      </c>
+      <c r="K254">
+        <v>15</v>
+      </c>
+      <c r="M254">
+        <f>-0.032*K254^4 + 2.1224*K254^3 - 43.522*K254^2 + 210.64*K254 + 1813.9</f>
+        <v>724.15000000000055</v>
+      </c>
+    </row>
+    <row r="255" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F255">
+        <v>9.5</v>
+      </c>
+      <c r="G255">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="256" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F256">
+        <v>12.5</v>
+      </c>
+      <c r="G256">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="257" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F257">
+        <v>15.5</v>
+      </c>
+      <c r="G257">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="258" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F258">
+        <v>24.5</v>
+      </c>
+      <c r="G258">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="259" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F259">
+        <v>30.5</v>
+      </c>
+      <c r="G259">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
PDS V1.3 DMA BIEN5
</commit_message>
<xml_diff>
--- a/STM32F051C8T6/MIS PROYECTOS/PORTABLE DIGITAL SOURCE V1.3 DMA/DESIGN POWER3.xlsx
+++ b/STM32F051C8T6/MIS PROYECTOS/PORTABLE DIGITAL SOURCE V1.3 DMA/DESIGN POWER3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIOVANNY_TODO\SKETCHS\STM32\STM32F051C8T6\MIS PROYECTOS\PORTABLE DIGITAL SOURCE V1.3 DMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F6C0EF-F02B-450C-92A5-74E6992C75EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B79E79-5330-4C1F-856E-1781621259FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97884494-F9FC-454E-B7F0-C1DF6E6FC067}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Vref</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Freq Deseada</t>
+  </si>
+  <si>
+    <t>LIMITE DE CORRIENTE</t>
   </si>
 </sst>
 </file>
@@ -1575,66 +1578,210 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$F$252:$F$259</c:f>
+              <c:f>Hoja1!$H$258:$H$289</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>30.5</c:v>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$G$252:$G$259</c:f>
+              <c:f>Hoja1!$I$258:$I$289</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>2100</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2050</c:v>
+                  <c:v>2450</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1250</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="16">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1642,7 +1789,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3392-49F9-BE21-23F3B66D58C2}"/>
+              <c16:uniqueId val="{00000000-DE92-46C0-8628-FA0A2AB6B0CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1654,11 +1801,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166230016"/>
-        <c:axId val="165899840"/>
+        <c:axId val="251324400"/>
+        <c:axId val="32370832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166230016"/>
+        <c:axId val="251324400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,12 +1862,12 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165899840"/>
+        <c:crossAx val="32370832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165899840"/>
+        <c:axId val="32370832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1924,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="166230016"/>
+        <c:crossAx val="251324400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3969,23 +4116,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>236</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>250</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 9">
+        <xdr:cNvPr id="15" name="Gráfico 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87212DC3-2CF3-4614-9FC4-4A271647C1FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38023575-9351-46DE-8856-DDA3C8C1ECD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4303,10 +4450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D153B7-22F3-48BB-9E72-85FF6508B366}">
-  <dimension ref="B6:Y259"/>
+  <dimension ref="B6:Y289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G241" sqref="G241"/>
+    <sheetView tabSelected="1" topLeftCell="A252" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G256" sqref="G256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,144 +7434,272 @@
         <v>43</v>
       </c>
     </row>
-    <row r="241" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F241">
+    <row r="256" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="258" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H258">
+        <v>0.1</v>
+      </c>
+      <c r="I258">
+        <v>2500</v>
+      </c>
+      <c r="L258">
+        <v>15</v>
+      </c>
+      <c r="M258">
+        <f>-0.012*L258^4 + 0.7163*L258^3 - 11.064*L258^2 - 59*L258 + 2541.3</f>
+        <v>976.91250000000036</v>
+      </c>
+    </row>
+    <row r="259" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H259">
         <v>1</v>
       </c>
-    </row>
-    <row r="242" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F242">
+      <c r="I259">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="260" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H260">
         <v>1.8</v>
       </c>
-      <c r="G242">
+      <c r="I260">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="261" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H261">
+        <v>2.5</v>
+      </c>
+      <c r="I261">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="262" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H262">
+        <v>3.3</v>
+      </c>
+      <c r="I262">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="263" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H263">
+        <v>4</v>
+      </c>
+      <c r="I263">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="264" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H264">
+        <v>5</v>
+      </c>
+      <c r="I264">
         <v>2200</v>
       </c>
     </row>
-    <row r="243" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F243">
-        <v>3.3</v>
-      </c>
-      <c r="G243">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="244" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F244">
-        <v>5</v>
-      </c>
-      <c r="G244">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="245" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F245">
+    <row r="265" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H265">
+        <v>6</v>
+      </c>
+      <c r="I265">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="266" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H266">
+        <v>7</v>
+      </c>
+      <c r="I266">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="267" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H267">
+        <v>8</v>
+      </c>
+      <c r="I267">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="268" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H268">
         <v>9</v>
       </c>
-      <c r="G245">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="246" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F246">
+      <c r="I268">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="269" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H269">
+        <v>10</v>
+      </c>
+      <c r="I269">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="270" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H270">
+        <v>11</v>
+      </c>
+      <c r="I270">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="271" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H271">
         <v>12</v>
       </c>
-      <c r="G246">
+      <c r="I271">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="272" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H272">
+        <v>13</v>
+      </c>
+      <c r="I272">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="273" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H273">
+        <v>14</v>
+      </c>
+      <c r="I273">
         <v>1000</v>
       </c>
     </row>
-    <row r="247" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F247">
+    <row r="274" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H274">
         <v>15</v>
       </c>
-      <c r="G247">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="248" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F248">
+      <c r="I274">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="275" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H275">
+        <v>16</v>
+      </c>
+      <c r="I275">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="276" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H276">
+        <v>17</v>
+      </c>
+      <c r="I276">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="277" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H277">
+        <v>18</v>
+      </c>
+      <c r="I277">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="278" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H278">
+        <v>19</v>
+      </c>
+      <c r="I278">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="279" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H279">
+        <v>20</v>
+      </c>
+      <c r="I279">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="280" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H280">
+        <v>21</v>
+      </c>
+      <c r="I280">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="281" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H281">
+        <v>22</v>
+      </c>
+      <c r="I281">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="282" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H282">
+        <v>23</v>
+      </c>
+      <c r="I282">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="283" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H283">
         <v>24</v>
       </c>
-      <c r="G248">
+      <c r="I283">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="284" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H284">
+        <v>25</v>
+      </c>
+      <c r="I284">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="285" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H285">
+        <v>26</v>
+      </c>
+      <c r="I285">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="286" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H286">
+        <v>27</v>
+      </c>
+      <c r="I286">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="287" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H287">
+        <v>28</v>
+      </c>
+      <c r="I287">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="288" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H288">
+        <v>29</v>
+      </c>
+      <c r="I288">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="289" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H289">
+        <v>30</v>
+      </c>
+      <c r="I289">
         <v>500</v>
-      </c>
-    </row>
-    <row r="249" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F249">
-        <v>30</v>
-      </c>
-      <c r="G249">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="252" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F252">
-        <v>2.5</v>
-      </c>
-      <c r="G252">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="253" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F253">
-        <v>3.8</v>
-      </c>
-      <c r="G253">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="254" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F254">
-        <v>7</v>
-      </c>
-      <c r="G254">
-        <v>2000</v>
-      </c>
-      <c r="K254">
-        <v>15</v>
-      </c>
-      <c r="M254">
-        <f>-0.032*K254^4 + 2.1224*K254^3 - 43.522*K254^2 + 210.64*K254 + 1813.9</f>
-        <v>724.15000000000055</v>
-      </c>
-    </row>
-    <row r="255" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F255">
-        <v>9.5</v>
-      </c>
-      <c r="G255">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="256" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F256">
-        <v>12.5</v>
-      </c>
-      <c r="G256">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="257" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F257">
-        <v>15.5</v>
-      </c>
-      <c r="G257">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="258" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F258">
-        <v>24.5</v>
-      </c>
-      <c r="G258">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="259" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F259">
-        <v>30.5</v>
-      </c>
-      <c r="G259">
-        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>